<commit_message>
Add new project analyzation and output files for .md update.
</commit_message>
<xml_diff>
--- a/NIS_Outputs.xlsx
+++ b/NIS_Outputs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6675" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6675" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="NIS_Outputs" sheetId="1" r:id="rId1"/>
@@ -1451,6 +1451,7 @@
               <a:solidFill>
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
+              <a:prstDash val="dash"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -2227,6 +2228,7 @@
               <a:solidFill>
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
+              <a:prstDash val="dash"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -3004,11 +3006,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="383871688"/>
-        <c:axId val="383871296"/>
+        <c:axId val="504601808"/>
+        <c:axId val="504598672"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="383871688"/>
+        <c:axId val="504601808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3050,7 +3052,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="383871296"/>
+        <c:crossAx val="504598672"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3058,7 +3060,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="383871296"/>
+        <c:axId val="504598672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3109,7 +3111,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="383871688"/>
+        <c:crossAx val="504601808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4021,6 +4023,7 @@
               <a:solidFill>
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
+              <a:prstDash val="dash"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -4794,6 +4797,7 @@
               <a:solidFill>
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
+              <a:prstDash val="dash"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -5568,11 +5572,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="532748392"/>
-        <c:axId val="532748784"/>
+        <c:axId val="504600240"/>
+        <c:axId val="504602200"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="532748392"/>
+        <c:axId val="504600240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5614,7 +5618,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="532748784"/>
+        <c:crossAx val="504602200"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5622,7 +5626,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="532748784"/>
+        <c:axId val="504602200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5673,7 +5677,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="532748392"/>
+        <c:crossAx val="504600240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7456,11 +7460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:B500"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B500"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -7481,7 +7484,7 @@
         <v>75.059700000000007</v>
       </c>
     </row>
-    <row r="3" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -7497,7 +7500,7 @@
         <v>3.02854</v>
       </c>
     </row>
-    <row r="5" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -7513,7 +7516,7 @@
         <v>5.8786800000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -7529,7 +7532,7 @@
         <v>6.7276800000000003</v>
       </c>
     </row>
-    <row r="9" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -7545,7 +7548,7 @@
         <v>0.35289900000000002</v>
       </c>
     </row>
-    <row r="11" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -7561,7 +7564,7 @@
         <v>1.7407999999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -7577,7 +7580,7 @@
         <v>2.97119</v>
       </c>
     </row>
-    <row r="15" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -7593,7 +7596,7 @@
         <v>1.74136</v>
       </c>
     </row>
-    <row r="17" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>0</v>
       </c>
@@ -7609,7 +7612,7 @@
         <v>2.78803</v>
       </c>
     </row>
-    <row r="19" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>0</v>
       </c>
@@ -7625,7 +7628,7 @@
         <v>1.4500599999999999</v>
       </c>
     </row>
-    <row r="21" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>0</v>
       </c>
@@ -7641,7 +7644,7 @@
         <v>5.1052600000000004</v>
       </c>
     </row>
-    <row r="23" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>0</v>
       </c>
@@ -7657,7 +7660,7 @@
         <v>0.87429699999999999</v>
       </c>
     </row>
-    <row r="25" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>0</v>
       </c>
@@ -7673,7 +7676,7 @@
         <v>4.42401</v>
       </c>
     </row>
-    <row r="27" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>0</v>
       </c>
@@ -7689,7 +7692,7 @@
         <v>3.4957799999999999</v>
       </c>
     </row>
-    <row r="29" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>0</v>
       </c>
@@ -7705,7 +7708,7 @@
         <v>2.93689</v>
       </c>
     </row>
-    <row r="31" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>0</v>
       </c>
@@ -7721,7 +7724,7 @@
         <v>5.8804800000000004</v>
       </c>
     </row>
-    <row r="33" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>0</v>
       </c>
@@ -7737,7 +7740,7 @@
         <v>6.3692399999999996</v>
       </c>
     </row>
-    <row r="35" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>0</v>
       </c>
@@ -7753,7 +7756,7 @@
         <v>4.1383999999999999</v>
       </c>
     </row>
-    <row r="37" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>0</v>
       </c>
@@ -7769,7 +7772,7 @@
         <v>4.4943400000000002</v>
       </c>
     </row>
-    <row r="39" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>0</v>
       </c>
@@ -7785,7 +7788,7 @@
         <v>4.3842499999999998</v>
       </c>
     </row>
-    <row r="41" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
         <v>0</v>
       </c>
@@ -7801,7 +7804,7 @@
         <v>1.74353</v>
       </c>
     </row>
-    <row r="43" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
         <v>0</v>
       </c>
@@ -7817,7 +7820,7 @@
         <v>1.23929</v>
       </c>
     </row>
-    <row r="45" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
         <v>0</v>
       </c>
@@ -7833,7 +7836,7 @@
         <v>1.0738799999999999</v>
       </c>
     </row>
-    <row r="47" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
         <v>0</v>
       </c>
@@ -7849,7 +7852,7 @@
         <v>0.93812700000000004</v>
       </c>
     </row>
-    <row r="49" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
         <v>0</v>
       </c>
@@ -7865,7 +7868,7 @@
         <v>3.47546</v>
       </c>
     </row>
-    <row r="51" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
         <v>0</v>
       </c>
@@ -7881,7 +7884,7 @@
         <v>10.849500000000001</v>
       </c>
     </row>
-    <row r="53" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
         <v>0</v>
       </c>
@@ -7897,7 +7900,7 @@
         <v>0.25043100000000001</v>
       </c>
     </row>
-    <row r="55" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
         <v>0</v>
       </c>
@@ -7913,7 +7916,7 @@
         <v>1.6053500000000001</v>
       </c>
     </row>
-    <row r="57" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
         <v>0</v>
       </c>
@@ -7929,7 +7932,7 @@
         <v>3.8650799999999998</v>
       </c>
     </row>
-    <row r="59" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
         <v>0</v>
       </c>
@@ -7945,7 +7948,7 @@
         <v>2.3863300000000001</v>
       </c>
     </row>
-    <row r="61" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
         <v>0</v>
       </c>
@@ -7961,7 +7964,7 @@
         <v>0.97967499999999996</v>
       </c>
     </row>
-    <row r="63" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
         <v>0</v>
       </c>
@@ -7977,7 +7980,7 @@
         <v>1.7034499999999999</v>
       </c>
     </row>
-    <row r="65" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
         <v>0</v>
       </c>
@@ -7993,7 +7996,7 @@
         <v>0.69567900000000005</v>
       </c>
     </row>
-    <row r="67" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
         <v>0</v>
       </c>
@@ -8009,7 +8012,7 @@
         <v>4.6342800000000004</v>
       </c>
     </row>
-    <row r="69" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
         <v>0</v>
       </c>
@@ -8025,7 +8028,7 @@
         <v>1.84653</v>
       </c>
     </row>
-    <row r="71" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
         <v>0</v>
       </c>
@@ -8041,7 +8044,7 @@
         <v>3.50359</v>
       </c>
     </row>
-    <row r="73" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
         <v>0</v>
       </c>
@@ -8057,7 +8060,7 @@
         <v>1.28111</v>
       </c>
     </row>
-    <row r="75" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
         <v>0</v>
       </c>
@@ -8073,7 +8076,7 @@
         <v>0.54807799999999995</v>
       </c>
     </row>
-    <row r="77" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
         <v>0</v>
       </c>
@@ -8089,7 +8092,7 @@
         <v>0.20009199999999999</v>
       </c>
     </row>
-    <row r="79" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A79" t="s">
         <v>0</v>
       </c>
@@ -8105,7 +8108,7 @@
         <v>0.53454000000000002</v>
       </c>
     </row>
-    <row r="81" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A81" t="s">
         <v>0</v>
       </c>
@@ -8121,7 +8124,7 @@
         <v>4.55185</v>
       </c>
     </row>
-    <row r="83" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A83" t="s">
         <v>0</v>
       </c>
@@ -8137,7 +8140,7 @@
         <v>0.38777899999999998</v>
       </c>
     </row>
-    <row r="85" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A85" t="s">
         <v>0</v>
       </c>
@@ -8153,7 +8156,7 @@
         <v>2.4836200000000002</v>
       </c>
     </row>
-    <row r="87" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A87" t="s">
         <v>0</v>
       </c>
@@ -8169,7 +8172,7 @@
         <v>0.80140599999999995</v>
       </c>
     </row>
-    <row r="89" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A89" t="s">
         <v>0</v>
       </c>
@@ -8185,7 +8188,7 @@
         <v>1.03302</v>
       </c>
     </row>
-    <row r="91" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A91" t="s">
         <v>0</v>
       </c>
@@ -8201,7 +8204,7 @@
         <v>2.8852600000000002</v>
       </c>
     </row>
-    <row r="93" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A93" t="s">
         <v>0</v>
       </c>
@@ -8217,7 +8220,7 @@
         <v>6.7239399999999998</v>
       </c>
     </row>
-    <row r="95" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A95" t="s">
         <v>0</v>
       </c>
@@ -8233,7 +8236,7 @@
         <v>2.9109699999999998</v>
       </c>
     </row>
-    <row r="97" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A97" t="s">
         <v>0</v>
       </c>
@@ -8249,7 +8252,7 @@
         <v>4.7422199999999997</v>
       </c>
     </row>
-    <row r="99" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A99" t="s">
         <v>0</v>
       </c>
@@ -8265,7 +8268,7 @@
         <v>10.410399999999999</v>
       </c>
     </row>
-    <row r="101" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A101" t="s">
         <v>0</v>
       </c>
@@ -8281,7 +8284,7 @@
         <v>3.9277600000000001</v>
       </c>
     </row>
-    <row r="103" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A103" t="s">
         <v>0</v>
       </c>
@@ -8297,7 +8300,7 @@
         <v>3.0931799999999998</v>
       </c>
     </row>
-    <row r="105" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A105" t="s">
         <v>0</v>
       </c>
@@ -8313,7 +8316,7 @@
         <v>2.1379100000000002</v>
       </c>
     </row>
-    <row r="107" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A107" t="s">
         <v>0</v>
       </c>
@@ -8329,7 +8332,7 @@
         <v>1.3535999999999999</v>
       </c>
     </row>
-    <row r="109" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A109" t="s">
         <v>0</v>
       </c>
@@ -8345,7 +8348,7 @@
         <v>0.85578500000000002</v>
       </c>
     </row>
-    <row r="111" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A111" t="s">
         <v>0</v>
       </c>
@@ -8361,7 +8364,7 @@
         <v>1.4061999999999999</v>
       </c>
     </row>
-    <row r="113" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A113" t="s">
         <v>0</v>
       </c>
@@ -8377,7 +8380,7 @@
         <v>3.4676499999999999</v>
       </c>
     </row>
-    <row r="115" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A115" t="s">
         <v>0</v>
       </c>
@@ -8393,7 +8396,7 @@
         <v>7.6469399999999998</v>
       </c>
     </row>
-    <row r="117" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A117" t="s">
         <v>0</v>
       </c>
@@ -8409,7 +8412,7 @@
         <v>1.48421</v>
       </c>
     </row>
-    <row r="119" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A119" t="s">
         <v>0</v>
       </c>
@@ -8425,7 +8428,7 @@
         <v>1.96665</v>
       </c>
     </row>
-    <row r="121" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A121" t="s">
         <v>0</v>
       </c>
@@ -8441,7 +8444,7 @@
         <v>0.32196200000000003</v>
       </c>
     </row>
-    <row r="123" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A123" t="s">
         <v>0</v>
       </c>
@@ -8457,7 +8460,7 @@
         <v>6.1917999999999997</v>
       </c>
     </row>
-    <row r="125" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A125" t="s">
         <v>0</v>
       </c>
@@ -8473,7 +8476,7 @@
         <v>6.3043300000000002</v>
       </c>
     </row>
-    <row r="127" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A127" t="s">
         <v>0</v>
       </c>
@@ -8489,7 +8492,7 @@
         <v>2.26051</v>
       </c>
     </row>
-    <row r="129" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A129" t="s">
         <v>0</v>
       </c>
@@ -8505,7 +8508,7 @@
         <v>2.12649</v>
       </c>
     </row>
-    <row r="131" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A131" t="s">
         <v>0</v>
       </c>
@@ -8521,7 +8524,7 @@
         <v>6.65442</v>
       </c>
     </row>
-    <row r="133" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A133" t="s">
         <v>0</v>
       </c>
@@ -8537,7 +8540,7 @@
         <v>1.86094</v>
       </c>
     </row>
-    <row r="135" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A135" t="s">
         <v>0</v>
       </c>
@@ -8553,7 +8556,7 @@
         <v>2.9550299999999998</v>
       </c>
     </row>
-    <row r="137" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A137" t="s">
         <v>0</v>
       </c>
@@ -8569,7 +8572,7 @@
         <v>3.1867100000000002</v>
       </c>
     </row>
-    <row r="139" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A139" t="s">
         <v>0</v>
       </c>
@@ -8585,7 +8588,7 @@
         <v>10.133599999999999</v>
       </c>
     </row>
-    <row r="141" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A141" t="s">
         <v>0</v>
       </c>
@@ -8601,7 +8604,7 @@
         <v>3.17808</v>
       </c>
     </row>
-    <row r="143" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A143" t="s">
         <v>0</v>
       </c>
@@ -8617,7 +8620,7 @@
         <v>5.6809099999999999</v>
       </c>
     </row>
-    <row r="145" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A145" t="s">
         <v>0</v>
       </c>
@@ -8633,7 +8636,7 @@
         <v>2.2052</v>
       </c>
     </row>
-    <row r="147" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A147" t="s">
         <v>0</v>
       </c>
@@ -8649,7 +8652,7 @@
         <v>1.3664700000000001</v>
       </c>
     </row>
-    <row r="149" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A149" t="s">
         <v>0</v>
       </c>
@@ -8665,7 +8668,7 @@
         <v>0.38065500000000002</v>
       </c>
     </row>
-    <row r="151" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A151" t="s">
         <v>0</v>
       </c>
@@ -8681,7 +8684,7 @@
         <v>2.2391899999999998</v>
       </c>
     </row>
-    <row r="153" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A153" t="s">
         <v>0</v>
       </c>
@@ -8697,7 +8700,7 @@
         <v>1.7613799999999999</v>
       </c>
     </row>
-    <row r="155" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A155" t="s">
         <v>0</v>
       </c>
@@ -8713,7 +8716,7 @@
         <v>2.6510799999999999</v>
       </c>
     </row>
-    <row r="157" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A157" t="s">
         <v>0</v>
       </c>
@@ -8729,7 +8732,7 @@
         <v>0.89376500000000003</v>
       </c>
     </row>
-    <row r="159" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A159" t="s">
         <v>0</v>
       </c>
@@ -8745,7 +8748,7 @@
         <v>1.0570200000000001</v>
       </c>
     </row>
-    <row r="161" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="161" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A161" t="s">
         <v>0</v>
       </c>
@@ -8761,7 +8764,7 @@
         <v>4.1265799999999997</v>
       </c>
     </row>
-    <row r="163" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A163" t="s">
         <v>0</v>
       </c>
@@ -8777,7 +8780,7 @@
         <v>5.7412299999999998</v>
       </c>
     </row>
-    <row r="165" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="165" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A165" t="s">
         <v>0</v>
       </c>
@@ -8793,7 +8796,7 @@
         <v>1.00762</v>
       </c>
     </row>
-    <row r="167" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="167" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A167" t="s">
         <v>0</v>
       </c>
@@ -8809,7 +8812,7 @@
         <v>2.2059000000000002</v>
       </c>
     </row>
-    <row r="169" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="169" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A169" t="s">
         <v>0</v>
       </c>
@@ -8825,7 +8828,7 @@
         <v>1.53329</v>
       </c>
     </row>
-    <row r="171" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="171" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A171" t="s">
         <v>0</v>
       </c>
@@ -8841,7 +8844,7 @@
         <v>4.5633800000000004</v>
       </c>
     </row>
-    <row r="173" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="173" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A173" t="s">
         <v>0</v>
       </c>
@@ -8857,7 +8860,7 @@
         <v>0.13741500000000001</v>
       </c>
     </row>
-    <row r="175" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="175" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A175" t="s">
         <v>0</v>
       </c>
@@ -8873,7 +8876,7 @@
         <v>3.5478800000000001</v>
       </c>
     </row>
-    <row r="177" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="177" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A177" t="s">
         <v>0</v>
       </c>
@@ -8889,7 +8892,7 @@
         <v>0.22314800000000001</v>
       </c>
     </row>
-    <row r="179" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="179" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A179" t="s">
         <v>0</v>
       </c>
@@ -8905,7 +8908,7 @@
         <v>0.39102799999999999</v>
       </c>
     </row>
-    <row r="181" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="181" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A181" t="s">
         <v>0</v>
       </c>
@@ -8921,7 +8924,7 @@
         <v>2.7044700000000002</v>
       </c>
     </row>
-    <row r="183" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="183" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A183" t="s">
         <v>0</v>
       </c>
@@ -8937,7 +8940,7 @@
         <v>2.2582200000000001</v>
       </c>
     </row>
-    <row r="185" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="185" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A185" t="s">
         <v>0</v>
       </c>
@@ -8953,7 +8956,7 @@
         <v>1.69275</v>
       </c>
     </row>
-    <row r="187" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="187" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A187" t="s">
         <v>0</v>
       </c>
@@ -8969,7 +8972,7 @@
         <v>4.4637500000000001</v>
       </c>
     </row>
-    <row r="189" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="189" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A189" t="s">
         <v>0</v>
       </c>
@@ -8985,7 +8988,7 @@
         <v>1.49261</v>
       </c>
     </row>
-    <row r="191" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="191" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A191" t="s">
         <v>0</v>
       </c>
@@ -9001,7 +9004,7 @@
         <v>1.39628</v>
       </c>
     </row>
-    <row r="193" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A193" t="s">
         <v>0</v>
       </c>
@@ -9017,7 +9020,7 @@
         <v>6.9768100000000004</v>
       </c>
     </row>
-    <row r="195" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="195" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A195" t="s">
         <v>0</v>
       </c>
@@ -9033,7 +9036,7 @@
         <v>3.3909799999999999</v>
       </c>
     </row>
-    <row r="197" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="197" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A197" t="s">
         <v>0</v>
       </c>
@@ -9049,7 +9052,7 @@
         <v>2.47343</v>
       </c>
     </row>
-    <row r="199" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="199" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A199" t="s">
         <v>0</v>
       </c>
@@ -9065,7 +9068,7 @@
         <v>3.2431700000000001</v>
       </c>
     </row>
-    <row r="201" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="201" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A201" t="s">
         <v>0</v>
       </c>
@@ -9081,7 +9084,7 @@
         <v>2.03355</v>
       </c>
     </row>
-    <row r="203" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="203" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A203" t="s">
         <v>0</v>
       </c>
@@ -9097,7 +9100,7 @@
         <v>5.0559500000000002</v>
       </c>
     </row>
-    <row r="205" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="205" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A205" t="s">
         <v>0</v>
       </c>
@@ -9113,7 +9116,7 @@
         <v>1.0522199999999999</v>
       </c>
     </row>
-    <row r="207" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="207" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A207" t="s">
         <v>0</v>
       </c>
@@ -9129,7 +9132,7 @@
         <v>2.1646100000000001</v>
       </c>
     </row>
-    <row r="209" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="209" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A209" t="s">
         <v>0</v>
       </c>
@@ -9145,7 +9148,7 @@
         <v>0.93909200000000004</v>
       </c>
     </row>
-    <row r="211" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="211" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A211" t="s">
         <v>0</v>
       </c>
@@ -9161,7 +9164,7 @@
         <v>2.15503</v>
       </c>
     </row>
-    <row r="213" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="213" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A213" t="s">
         <v>0</v>
       </c>
@@ -9177,7 +9180,7 @@
         <v>1.8991499999999999</v>
       </c>
     </row>
-    <row r="215" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="215" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A215" t="s">
         <v>0</v>
       </c>
@@ -9193,7 +9196,7 @@
         <v>3.62751</v>
       </c>
     </row>
-    <row r="217" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="217" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A217" t="s">
         <v>0</v>
       </c>
@@ -9209,7 +9212,7 @@
         <v>1.1694899999999999</v>
       </c>
     </row>
-    <row r="219" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="219" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A219" t="s">
         <v>0</v>
       </c>
@@ -9225,7 +9228,7 @@
         <v>0.930114</v>
       </c>
     </row>
-    <row r="221" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="221" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A221" t="s">
         <v>0</v>
       </c>
@@ -9241,7 +9244,7 @@
         <v>3.7172299999999998</v>
       </c>
     </row>
-    <row r="223" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="223" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A223" t="s">
         <v>0</v>
       </c>
@@ -9257,7 +9260,7 @@
         <v>3.8162099999999999</v>
       </c>
     </row>
-    <row r="225" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="225" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A225" t="s">
         <v>0</v>
       </c>
@@ -9273,7 +9276,7 @@
         <v>2.7901699999999998</v>
       </c>
     </row>
-    <row r="227" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="227" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A227" t="s">
         <v>0</v>
       </c>
@@ -9289,7 +9292,7 @@
         <v>2.79494</v>
       </c>
     </row>
-    <row r="229" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="229" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A229" t="s">
         <v>0</v>
       </c>
@@ -9305,7 +9308,7 @@
         <v>1.54033</v>
       </c>
     </row>
-    <row r="231" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="231" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A231" t="s">
         <v>0</v>
       </c>
@@ -9321,7 +9324,7 @@
         <v>1.7941499999999999</v>
       </c>
     </row>
-    <row r="233" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="233" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A233" t="s">
         <v>0</v>
       </c>
@@ -9337,7 +9340,7 @@
         <v>0.40376499999999999</v>
       </c>
     </row>
-    <row r="235" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="235" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A235" t="s">
         <v>0</v>
       </c>
@@ -9353,7 +9356,7 @@
         <v>2.6479499999999998</v>
       </c>
     </row>
-    <row r="237" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="237" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A237" t="s">
         <v>0</v>
       </c>
@@ -9369,7 +9372,7 @@
         <v>1.6184099999999999</v>
       </c>
     </row>
-    <row r="239" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="239" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A239" t="s">
         <v>0</v>
       </c>
@@ -9385,7 +9388,7 @@
         <v>2.9986600000000001</v>
       </c>
     </row>
-    <row r="241" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="241" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A241" t="s">
         <v>0</v>
       </c>
@@ -9401,7 +9404,7 @@
         <v>5.3338599999999996</v>
       </c>
     </row>
-    <row r="243" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="243" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A243" t="s">
         <v>0</v>
       </c>
@@ -9417,7 +9420,7 @@
         <v>5.5711199999999996</v>
       </c>
     </row>
-    <row r="245" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="245" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A245" t="s">
         <v>0</v>
       </c>
@@ -9433,7 +9436,7 @@
         <v>1.63486</v>
       </c>
     </row>
-    <row r="247" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="247" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A247" t="s">
         <v>0</v>
       </c>
@@ -9449,7 +9452,7 @@
         <v>4.2413699999999999</v>
       </c>
     </row>
-    <row r="249" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="249" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A249" t="s">
         <v>0</v>
       </c>
@@ -9465,7 +9468,7 @@
         <v>3.0885500000000001</v>
       </c>
     </row>
-    <row r="251" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="251" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A251" t="s">
         <v>0</v>
       </c>
@@ -9481,7 +9484,7 @@
         <v>2.1235499999999998</v>
       </c>
     </row>
-    <row r="253" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="253" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A253" t="s">
         <v>0</v>
       </c>
@@ -9497,7 +9500,7 @@
         <v>0.30676700000000001</v>
       </c>
     </row>
-    <row r="255" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="255" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A255" t="s">
         <v>0</v>
       </c>
@@ -9513,7 +9516,7 @@
         <v>2.1951800000000001</v>
       </c>
     </row>
-    <row r="257" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="257" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A257" t="s">
         <v>0</v>
       </c>
@@ -9529,7 +9532,7 @@
         <v>1.1587099999999999</v>
       </c>
     </row>
-    <row r="259" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="259" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A259" t="s">
         <v>0</v>
       </c>
@@ -9545,7 +9548,7 @@
         <v>3.9504600000000001</v>
       </c>
     </row>
-    <row r="261" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="261" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A261" t="s">
         <v>0</v>
       </c>
@@ -9561,7 +9564,7 @@
         <v>0.75331599999999999</v>
       </c>
     </row>
-    <row r="263" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="263" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A263" t="s">
         <v>0</v>
       </c>
@@ -9577,7 +9580,7 @@
         <v>0.236175</v>
       </c>
     </row>
-    <row r="265" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="265" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A265" t="s">
         <v>0</v>
       </c>
@@ -9593,7 +9596,7 @@
         <v>3.8482599999999998</v>
       </c>
     </row>
-    <row r="267" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="267" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A267" t="s">
         <v>0</v>
       </c>
@@ -9609,7 +9612,7 @@
         <v>0.62130700000000005</v>
       </c>
     </row>
-    <row r="269" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="269" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A269" t="s">
         <v>0</v>
       </c>
@@ -9625,7 +9628,7 @@
         <v>0.97965899999999995</v>
       </c>
     </row>
-    <row r="271" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="271" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A271" t="s">
         <v>0</v>
       </c>
@@ -9641,7 +9644,7 @@
         <v>5.3920199999999996</v>
       </c>
     </row>
-    <row r="273" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="273" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A273" t="s">
         <v>0</v>
       </c>
@@ -9657,7 +9660,7 @@
         <v>5.9663300000000001</v>
       </c>
     </row>
-    <row r="275" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="275" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A275" t="s">
         <v>0</v>
       </c>
@@ -9673,7 +9676,7 @@
         <v>3.9964300000000001</v>
       </c>
     </row>
-    <row r="277" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="277" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A277" t="s">
         <v>0</v>
       </c>
@@ -9689,7 +9692,7 @@
         <v>5.2790600000000003</v>
       </c>
     </row>
-    <row r="279" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="279" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A279" t="s">
         <v>0</v>
       </c>
@@ -9705,7 +9708,7 @@
         <v>2.7388599999999999</v>
       </c>
     </row>
-    <row r="281" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="281" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A281" t="s">
         <v>0</v>
       </c>
@@ -9721,7 +9724,7 @@
         <v>4.0237499999999997</v>
       </c>
     </row>
-    <row r="283" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="283" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A283" t="s">
         <v>0</v>
       </c>
@@ -9737,7 +9740,7 @@
         <v>2.9732400000000001</v>
       </c>
     </row>
-    <row r="285" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="285" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A285" t="s">
         <v>0</v>
       </c>
@@ -9753,7 +9756,7 @@
         <v>1.04634</v>
       </c>
     </row>
-    <row r="287" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="287" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A287" t="s">
         <v>0</v>
       </c>
@@ -9769,7 +9772,7 @@
         <v>0.256166</v>
       </c>
     </row>
-    <row r="289" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="289" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A289" t="s">
         <v>0</v>
       </c>
@@ -9785,7 +9788,7 @@
         <v>4.4655899999999997</v>
       </c>
     </row>
-    <row r="291" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="291" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A291" t="s">
         <v>0</v>
       </c>
@@ -9801,7 +9804,7 @@
         <v>0.46405400000000002</v>
       </c>
     </row>
-    <row r="293" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="293" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A293" t="s">
         <v>0</v>
       </c>
@@ -9817,7 +9820,7 @@
         <v>0.384658</v>
       </c>
     </row>
-    <row r="295" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="295" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A295" t="s">
         <v>0</v>
       </c>
@@ -9833,7 +9836,7 @@
         <v>2.5943900000000002</v>
       </c>
     </row>
-    <row r="297" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="297" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A297" t="s">
         <v>0</v>
       </c>
@@ -9849,7 +9852,7 @@
         <v>4.3268700000000004</v>
       </c>
     </row>
-    <row r="299" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="299" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A299" t="s">
         <v>0</v>
       </c>
@@ -9865,7 +9868,7 @@
         <v>0.426151</v>
       </c>
     </row>
-    <row r="301" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="301" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A301" t="s">
         <v>0</v>
       </c>
@@ -9881,7 +9884,7 @@
         <v>7.0597799999999999</v>
       </c>
     </row>
-    <row r="303" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="303" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A303" t="s">
         <v>0</v>
       </c>
@@ -9897,7 +9900,7 @@
         <v>0.88670899999999997</v>
       </c>
     </row>
-    <row r="305" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="305" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A305" t="s">
         <v>0</v>
       </c>
@@ -9913,7 +9916,7 @@
         <v>6.6559499999999998</v>
       </c>
     </row>
-    <row r="307" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="307" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A307" t="s">
         <v>0</v>
       </c>
@@ -9929,7 +9932,7 @@
         <v>1.1031</v>
       </c>
     </row>
-    <row r="309" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="309" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A309" t="s">
         <v>0</v>
       </c>
@@ -9945,7 +9948,7 @@
         <v>1.98495</v>
       </c>
     </row>
-    <row r="311" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="311" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A311" t="s">
         <v>0</v>
       </c>
@@ -9961,7 +9964,7 @@
         <v>1.3743700000000001</v>
       </c>
     </row>
-    <row r="313" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="313" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A313" t="s">
         <v>0</v>
       </c>
@@ -9977,7 +9980,7 @@
         <v>2.0375100000000002</v>
       </c>
     </row>
-    <row r="315" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="315" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A315" t="s">
         <v>0</v>
       </c>
@@ -9993,7 +9996,7 @@
         <v>2.4820099999999998</v>
       </c>
     </row>
-    <row r="317" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="317" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A317" t="s">
         <v>0</v>
       </c>
@@ -10009,7 +10012,7 @@
         <v>2.2635200000000002</v>
       </c>
     </row>
-    <row r="319" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="319" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A319" t="s">
         <v>0</v>
       </c>
@@ -10025,7 +10028,7 @@
         <v>2.18581</v>
       </c>
     </row>
-    <row r="321" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="321" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A321" t="s">
         <v>0</v>
       </c>
@@ -10041,7 +10044,7 @@
         <v>2.4659499999999999</v>
       </c>
     </row>
-    <row r="323" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="323" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A323" t="s">
         <v>0</v>
       </c>
@@ -10057,7 +10060,7 @@
         <v>4.0384200000000003</v>
       </c>
     </row>
-    <row r="325" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="325" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A325" t="s">
         <v>0</v>
       </c>
@@ -10073,7 +10076,7 @@
         <v>2.7684799999999998</v>
       </c>
     </row>
-    <row r="327" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="327" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A327" t="s">
         <v>0</v>
       </c>
@@ -10089,7 +10092,7 @@
         <v>0.26141700000000001</v>
       </c>
     </row>
-    <row r="329" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="329" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A329" t="s">
         <v>0</v>
       </c>
@@ -10105,7 +10108,7 @@
         <v>4.4794499999999999</v>
       </c>
     </row>
-    <row r="331" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="331" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A331" t="s">
         <v>0</v>
       </c>
@@ -10121,7 +10124,7 @@
         <v>1.9075800000000001</v>
       </c>
     </row>
-    <row r="333" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="333" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A333" t="s">
         <v>0</v>
       </c>
@@ -10137,7 +10140,7 @@
         <v>2.2671600000000001</v>
       </c>
     </row>
-    <row r="335" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="335" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A335" t="s">
         <v>0</v>
       </c>
@@ -10153,7 +10156,7 @@
         <v>5.2255700000000003</v>
       </c>
     </row>
-    <row r="337" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="337" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A337" t="s">
         <v>0</v>
       </c>
@@ -10169,7 +10172,7 @@
         <v>7.9648500000000002</v>
       </c>
     </row>
-    <row r="339" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="339" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A339" t="s">
         <v>0</v>
       </c>
@@ -10185,7 +10188,7 @@
         <v>1.68858</v>
       </c>
     </row>
-    <row r="341" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="341" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A341" t="s">
         <v>0</v>
       </c>
@@ -10201,7 +10204,7 @@
         <v>0.68205400000000005</v>
       </c>
     </row>
-    <row r="343" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="343" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A343" t="s">
         <v>0</v>
       </c>
@@ -10217,7 +10220,7 @@
         <v>1.6936800000000001</v>
       </c>
     </row>
-    <row r="345" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="345" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A345" t="s">
         <v>0</v>
       </c>
@@ -10233,7 +10236,7 @@
         <v>3.9838200000000001</v>
       </c>
     </row>
-    <row r="347" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="347" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A347" t="s">
         <v>0</v>
       </c>
@@ -10249,7 +10252,7 @@
         <v>1.10599</v>
       </c>
     </row>
-    <row r="349" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="349" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A349" t="s">
         <v>0</v>
       </c>
@@ -10265,7 +10268,7 @@
         <v>4.91214</v>
       </c>
     </row>
-    <row r="351" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="351" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A351" t="s">
         <v>0</v>
       </c>
@@ -10281,7 +10284,7 @@
         <v>1.52851</v>
       </c>
     </row>
-    <row r="353" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="353" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A353" t="s">
         <v>0</v>
       </c>
@@ -10297,7 +10300,7 @@
         <v>2.3206199999999999</v>
       </c>
     </row>
-    <row r="355" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="355" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A355" t="s">
         <v>0</v>
       </c>
@@ -10313,7 +10316,7 @@
         <v>1.81569</v>
       </c>
     </row>
-    <row r="357" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="357" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A357" t="s">
         <v>0</v>
       </c>
@@ -10329,7 +10332,7 @@
         <v>6.6258600000000003</v>
       </c>
     </row>
-    <row r="359" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="359" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A359" t="s">
         <v>0</v>
       </c>
@@ -10345,7 +10348,7 @@
         <v>1.91856</v>
       </c>
     </row>
-    <row r="361" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="361" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A361" t="s">
         <v>0</v>
       </c>
@@ -10361,7 +10364,7 @@
         <v>1.0605199999999999</v>
       </c>
     </row>
-    <row r="363" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="363" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A363" t="s">
         <v>0</v>
       </c>
@@ -10377,7 +10380,7 @@
         <v>3.3841600000000001</v>
       </c>
     </row>
-    <row r="365" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="365" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A365" t="s">
         <v>0</v>
       </c>
@@ -10393,7 +10396,7 @@
         <v>1.8675200000000001</v>
       </c>
     </row>
-    <row r="367" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="367" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A367" t="s">
         <v>0</v>
       </c>
@@ -10409,7 +10412,7 @@
         <v>0.916771</v>
       </c>
     </row>
-    <row r="369" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="369" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A369" t="s">
         <v>0</v>
       </c>
@@ -10425,7 +10428,7 @@
         <v>1.89018</v>
       </c>
     </row>
-    <row r="371" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="371" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A371" t="s">
         <v>0</v>
       </c>
@@ -10441,7 +10444,7 @@
         <v>3.4389599999999998</v>
       </c>
     </row>
-    <row r="373" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="373" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A373" t="s">
         <v>0</v>
       </c>
@@ -10457,7 +10460,7 @@
         <v>0.31905</v>
       </c>
     </row>
-    <row r="375" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="375" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A375" t="s">
         <v>0</v>
       </c>
@@ -10473,7 +10476,7 @@
         <v>1.85884</v>
       </c>
     </row>
-    <row r="377" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="377" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A377" t="s">
         <v>0</v>
       </c>
@@ -10489,7 +10492,7 @@
         <v>1.3204899999999999</v>
       </c>
     </row>
-    <row r="379" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="379" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A379" t="s">
         <v>0</v>
       </c>
@@ -10505,7 +10508,7 @@
         <v>6.3770699999999998</v>
       </c>
     </row>
-    <row r="381" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="381" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A381" t="s">
         <v>0</v>
       </c>
@@ -10521,7 +10524,7 @@
         <v>0.18348400000000001</v>
       </c>
     </row>
-    <row r="383" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="383" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A383" t="s">
         <v>0</v>
       </c>
@@ -10537,7 +10540,7 @@
         <v>11.1541</v>
       </c>
     </row>
-    <row r="385" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="385" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A385" t="s">
         <v>0</v>
       </c>
@@ -10553,7 +10556,7 @@
         <v>3.4959699999999998</v>
       </c>
     </row>
-    <row r="387" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="387" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A387" t="s">
         <v>0</v>
       </c>
@@ -10569,7 +10572,7 @@
         <v>0.43506</v>
       </c>
     </row>
-    <row r="389" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="389" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A389" t="s">
         <v>0</v>
       </c>
@@ -10585,7 +10588,7 @@
         <v>1.44387</v>
       </c>
     </row>
-    <row r="391" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="391" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A391" t="s">
         <v>0</v>
       </c>
@@ -10601,7 +10604,7 @@
         <v>1.05139</v>
       </c>
     </row>
-    <row r="393" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="393" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A393" t="s">
         <v>0</v>
       </c>
@@ -10617,7 +10620,7 @@
         <v>1.9982599999999999</v>
       </c>
     </row>
-    <row r="395" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="395" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A395" t="s">
         <v>0</v>
       </c>
@@ -10633,7 +10636,7 @@
         <v>1.7020299999999999</v>
       </c>
     </row>
-    <row r="397" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="397" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A397" t="s">
         <v>0</v>
       </c>
@@ -10649,7 +10652,7 @@
         <v>5.20695</v>
       </c>
     </row>
-    <row r="399" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="399" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A399" t="s">
         <v>0</v>
       </c>
@@ -10665,7 +10668,7 @@
         <v>2.2018300000000002</v>
       </c>
     </row>
-    <row r="401" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="401" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A401" t="s">
         <v>0</v>
       </c>
@@ -10681,7 +10684,7 @@
         <v>1.74946</v>
       </c>
     </row>
-    <row r="403" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="403" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A403" t="s">
         <v>0</v>
       </c>
@@ -10697,7 +10700,7 @@
         <v>1.7640800000000001</v>
       </c>
     </row>
-    <row r="405" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="405" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A405" t="s">
         <v>0</v>
       </c>
@@ -10713,7 +10716,7 @@
         <v>7.1443500000000002</v>
       </c>
     </row>
-    <row r="407" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="407" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A407" t="s">
         <v>0</v>
       </c>
@@ -10729,7 +10732,7 @@
         <v>8.0645299999999995</v>
       </c>
     </row>
-    <row r="409" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="409" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A409" t="s">
         <v>0</v>
       </c>
@@ -10745,7 +10748,7 @@
         <v>0.26712399999999997</v>
       </c>
     </row>
-    <row r="411" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="411" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A411" t="s">
         <v>0</v>
       </c>
@@ -10761,7 +10764,7 @@
         <v>0.69036399999999998</v>
       </c>
     </row>
-    <row r="413" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="413" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A413" t="s">
         <v>0</v>
       </c>
@@ -10777,7 +10780,7 @@
         <v>3.01518</v>
       </c>
     </row>
-    <row r="415" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="415" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A415" t="s">
         <v>0</v>
       </c>
@@ -10793,7 +10796,7 @@
         <v>2.1389900000000002</v>
       </c>
     </row>
-    <row r="417" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="417" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A417" t="s">
         <v>0</v>
       </c>
@@ -10809,7 +10812,7 @@
         <v>1.11416</v>
       </c>
     </row>
-    <row r="419" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="419" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A419" t="s">
         <v>0</v>
       </c>
@@ -10825,7 +10828,7 @@
         <v>0.61617900000000003</v>
       </c>
     </row>
-    <row r="421" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="421" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A421" t="s">
         <v>0</v>
       </c>
@@ -10841,7 +10844,7 @@
         <v>8.9688499999999998</v>
       </c>
     </row>
-    <row r="423" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="423" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A423" t="s">
         <v>0</v>
       </c>
@@ -10857,7 +10860,7 @@
         <v>2.3142</v>
       </c>
     </row>
-    <row r="425" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="425" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A425" t="s">
         <v>0</v>
       </c>
@@ -10873,7 +10876,7 @@
         <v>0.92461800000000005</v>
       </c>
     </row>
-    <row r="427" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="427" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A427" t="s">
         <v>0</v>
       </c>
@@ -10889,7 +10892,7 @@
         <v>3.1561599999999999</v>
       </c>
     </row>
-    <row r="429" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="429" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A429" t="s">
         <v>0</v>
       </c>
@@ -10905,7 +10908,7 @@
         <v>4.8482900000000004</v>
       </c>
     </row>
-    <row r="431" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="431" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A431" t="s">
         <v>0</v>
       </c>
@@ -10921,7 +10924,7 @@
         <v>1.82284</v>
       </c>
     </row>
-    <row r="433" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="433" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A433" t="s">
         <v>0</v>
       </c>
@@ -10937,7 +10940,7 @@
         <v>5.52515</v>
       </c>
     </row>
-    <row r="435" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="435" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A435" t="s">
         <v>0</v>
       </c>
@@ -10953,7 +10956,7 @@
         <v>1.5821099999999999</v>
       </c>
     </row>
-    <row r="437" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="437" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A437" t="s">
         <v>0</v>
       </c>
@@ -10969,7 +10972,7 @@
         <v>2.6851699999999998</v>
       </c>
     </row>
-    <row r="439" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="439" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A439" t="s">
         <v>0</v>
       </c>
@@ -10985,7 +10988,7 @@
         <v>5.75793</v>
       </c>
     </row>
-    <row r="441" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="441" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A441" t="s">
         <v>0</v>
       </c>
@@ -11001,7 +11004,7 @@
         <v>1.55775</v>
       </c>
     </row>
-    <row r="443" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="443" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A443" t="s">
         <v>0</v>
       </c>
@@ -11017,7 +11020,7 @@
         <v>6.2821600000000002</v>
       </c>
     </row>
-    <row r="445" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="445" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A445" t="s">
         <v>0</v>
       </c>
@@ -11033,7 +11036,7 @@
         <v>4.4747300000000001</v>
       </c>
     </row>
-    <row r="447" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="447" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A447" t="s">
         <v>0</v>
       </c>
@@ -11049,7 +11052,7 @@
         <v>1.6826000000000001</v>
       </c>
     </row>
-    <row r="449" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="449" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A449" t="s">
         <v>0</v>
       </c>
@@ -11065,7 +11068,7 @@
         <v>1.2934099999999999</v>
       </c>
     </row>
-    <row r="451" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="451" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A451" t="s">
         <v>0</v>
       </c>
@@ -11081,7 +11084,7 @@
         <v>4.40632</v>
       </c>
     </row>
-    <row r="453" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="453" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A453" t="s">
         <v>0</v>
       </c>
@@ -11097,7 +11100,7 @@
         <v>1.67886</v>
       </c>
     </row>
-    <row r="455" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="455" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A455" t="s">
         <v>0</v>
       </c>
@@ -11113,7 +11116,7 @@
         <v>6.0205000000000002</v>
       </c>
     </row>
-    <row r="457" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="457" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A457" t="s">
         <v>0</v>
       </c>
@@ -11129,7 +11132,7 @@
         <v>2.88733</v>
       </c>
     </row>
-    <row r="459" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="459" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A459" t="s">
         <v>0</v>
       </c>
@@ -11145,7 +11148,7 @@
         <v>0.52253400000000005</v>
       </c>
     </row>
-    <row r="461" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="461" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A461" t="s">
         <v>0</v>
       </c>
@@ -11161,7 +11164,7 @@
         <v>0.127106</v>
       </c>
     </row>
-    <row r="463" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="463" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A463" t="s">
         <v>0</v>
       </c>
@@ -11177,7 +11180,7 @@
         <v>0.66895499999999997</v>
       </c>
     </row>
-    <row r="465" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="465" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A465" t="s">
         <v>0</v>
       </c>
@@ -11193,7 +11196,7 @@
         <v>0.246227</v>
       </c>
     </row>
-    <row r="467" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="467" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A467" t="s">
         <v>0</v>
       </c>
@@ -11209,7 +11212,7 @@
         <v>8.1873000000000005</v>
       </c>
     </row>
-    <row r="469" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="469" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A469" t="s">
         <v>0</v>
       </c>
@@ -11225,7 +11228,7 @@
         <v>6.4476199999999997</v>
       </c>
     </row>
-    <row r="471" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="471" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A471" t="s">
         <v>0</v>
       </c>
@@ -11241,7 +11244,7 @@
         <v>0.65226399999999995</v>
       </c>
     </row>
-    <row r="473" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="473" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A473" t="s">
         <v>0</v>
       </c>
@@ -11257,7 +11260,7 @@
         <v>2.0783399999999999</v>
       </c>
     </row>
-    <row r="475" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="475" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A475" t="s">
         <v>0</v>
       </c>
@@ -11273,7 +11276,7 @@
         <v>0.27737400000000001</v>
       </c>
     </row>
-    <row r="477" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="477" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A477" t="s">
         <v>0</v>
       </c>
@@ -11289,7 +11292,7 @@
         <v>1.4313400000000001</v>
       </c>
     </row>
-    <row r="479" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="479" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A479" t="s">
         <v>0</v>
       </c>
@@ -11305,7 +11308,7 @@
         <v>0.558975</v>
       </c>
     </row>
-    <row r="481" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="481" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A481" t="s">
         <v>0</v>
       </c>
@@ -11321,7 +11324,7 @@
         <v>2.7814399999999999</v>
       </c>
     </row>
-    <row r="483" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="483" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A483" t="s">
         <v>0</v>
       </c>
@@ -11337,7 +11340,7 @@
         <v>9.9578100000000003</v>
       </c>
     </row>
-    <row r="485" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="485" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A485" t="s">
         <v>0</v>
       </c>
@@ -11353,7 +11356,7 @@
         <v>0.15425900000000001</v>
       </c>
     </row>
-    <row r="487" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="487" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A487" t="s">
         <v>0</v>
       </c>
@@ -11369,7 +11372,7 @@
         <v>6.7072700000000003</v>
       </c>
     </row>
-    <row r="489" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="489" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A489" t="s">
         <v>0</v>
       </c>
@@ -11385,7 +11388,7 @@
         <v>4.0922099999999997</v>
       </c>
     </row>
-    <row r="491" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="491" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A491" t="s">
         <v>0</v>
       </c>
@@ -11401,7 +11404,7 @@
         <v>2.74532</v>
       </c>
     </row>
-    <row r="493" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="493" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A493" t="s">
         <v>0</v>
       </c>
@@ -11417,7 +11420,7 @@
         <v>6.6361400000000001</v>
       </c>
     </row>
-    <row r="495" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="495" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A495" t="s">
         <v>0</v>
       </c>
@@ -11433,7 +11436,7 @@
         <v>1.3123</v>
       </c>
     </row>
-    <row r="497" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="497" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A497" t="s">
         <v>0</v>
       </c>
@@ -11449,7 +11452,7 @@
         <v>1.9609399999999999</v>
       </c>
     </row>
-    <row r="499" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="499" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A499" t="s">
         <v>0</v>
       </c>
@@ -11466,13 +11469,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:A500">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="R"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:A500"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -11481,8 +11478,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D250"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="V39" sqref="V39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T43" sqref="T43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -14997,8 +14994,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D250"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J42" sqref="J42"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="AB17" sqref="AB17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>